<commit_message>
CORRECTION IN SQL SCRIPT DIDH
</commit_message>
<xml_diff>
--- a/didh/excel/ot.xlsx
+++ b/didh/excel/ot.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\reco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev2\super-gen\didh\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="778" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CERD" sheetId="1" r:id="rId1"/>
@@ -4688,9 +4688,6 @@
     <t>3;28</t>
   </si>
   <si>
-    <t>15:1;10</t>
-  </si>
-  <si>
     <t>15;6</t>
   </si>
   <si>
@@ -5517,12 +5514,15 @@
   </si>
   <si>
     <t>6;6;8</t>
+  </si>
+  <si>
+    <t>15;1;10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6471,8 +6471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6596,7 +6596,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="132" t="s">
-        <v>1307</v>
+        <v>1582</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>29</v>
@@ -6628,7 +6628,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>31</v>
@@ -6852,7 +6852,7 @@
         <v>46</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>47</v>
@@ -6861,7 +6861,7 @@
         <v>1239</v>
       </c>
       <c r="I12" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>1236</v>
@@ -6884,7 +6884,7 @@
         <v>1240</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>56</v>
@@ -6904,10 +6904,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="38" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>1510</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>1511</v>
       </c>
       <c r="D14" s="38" t="s">
         <v>49</v>
@@ -6936,10 +6936,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="38" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>1512</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>1513</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>51</v>
@@ -6980,7 +6980,7 @@
         <v>53</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>62</v>
@@ -7067,7 +7067,7 @@
         <v>1244</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>70</v>
@@ -7084,10 +7084,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="38" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>66</v>
@@ -7096,7 +7096,7 @@
         <v>67</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>71</v>
@@ -7113,10 +7113,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="38" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C21" s="38" t="s">
         <v>1516</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>1517</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>73</v>
@@ -7154,7 +7154,7 @@
         <v>233</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>82</v>
@@ -7163,7 +7163,7 @@
         <v>1245</v>
       </c>
       <c r="I22" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -7192,7 +7192,7 @@
         <v>84</v>
       </c>
       <c r="I23" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7212,7 +7212,7 @@
         <v>79</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="G24" s="19" t="s">
         <v>85</v>
@@ -7221,7 +7221,7 @@
         <v>86</v>
       </c>
       <c r="I24" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7241,7 +7241,7 @@
         <v>88</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>89</v>
@@ -7270,7 +7270,7 @@
         <v>92</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>93</v>
@@ -7279,7 +7279,7 @@
         <v>94</v>
       </c>
       <c r="I26" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -7299,7 +7299,7 @@
         <v>96</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>99</v>
@@ -7328,7 +7328,7 @@
         <v>98</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>101</v>
@@ -7357,7 +7357,7 @@
         <v>1247</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>103</v>
@@ -7366,7 +7366,7 @@
         <v>104</v>
       </c>
       <c r="I29" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7386,7 +7386,7 @@
         <v>106</v>
       </c>
       <c r="F30" s="104" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>109</v>
@@ -7395,7 +7395,7 @@
         <v>110</v>
       </c>
       <c r="I30" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7415,7 +7415,7 @@
         <v>108</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>582</v>
@@ -7424,7 +7424,7 @@
         <v>1303</v>
       </c>
       <c r="I31" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7469,7 +7469,7 @@
         <v>114</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>117</v>
@@ -7491,8 +7491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7541,10 +7541,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>1518</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>1519</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>119</v>
@@ -7553,7 +7553,7 @@
         <v>1191</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>123</v>
@@ -7573,10 +7573,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>1518</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>1519</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>120</v>
@@ -7585,7 +7585,7 @@
         <v>1190</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>125</v>
@@ -7602,10 +7602,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>1518</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>1519</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>121</v>
@@ -7614,7 +7614,7 @@
         <v>1192</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>127</v>
@@ -7643,7 +7643,7 @@
         <v>130</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>128</v>
@@ -7672,7 +7672,7 @@
         <v>238</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="G6" s="57" t="s">
         <v>236</v>
@@ -7681,7 +7681,7 @@
         <v>237</v>
       </c>
       <c r="I6" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -7701,7 +7701,7 @@
         <v>239</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>141</v>
@@ -7730,7 +7730,7 @@
         <v>1194</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>142</v>
@@ -7747,10 +7747,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>1520</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1521</v>
       </c>
       <c r="D9" s="38" t="s">
         <v>134</v>
@@ -7759,7 +7759,7 @@
         <v>241</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>144</v>
@@ -7768,7 +7768,7 @@
         <v>145</v>
       </c>
       <c r="I9" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -7788,7 +7788,7 @@
         <v>242</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>146</v>
@@ -7797,7 +7797,7 @@
         <v>243</v>
       </c>
       <c r="I10" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -7817,7 +7817,7 @@
         <v>137</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>147</v>
@@ -7826,7 +7826,7 @@
         <v>148</v>
       </c>
       <c r="I11" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -7834,10 +7834,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>107</v>
@@ -7846,7 +7846,7 @@
         <v>245</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="G12" s="57" t="s">
         <v>149</v>
@@ -7855,7 +7855,7 @@
         <v>244</v>
       </c>
       <c r="I12" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -7863,10 +7863,10 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>138</v>
@@ -7875,7 +7875,7 @@
         <v>139</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="G13" s="57" t="s">
         <v>150</v>
@@ -7901,10 +7901,10 @@
         <v>140</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>151</v>
@@ -7921,10 +7921,10 @@
         <v>2</v>
       </c>
       <c r="B15" s="71" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C15" s="71" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D15" s="68" t="s">
         <v>1166</v>
@@ -7933,7 +7933,7 @@
         <v>1172</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="G15" s="70" t="s">
         <v>1167</v>
@@ -7950,10 +7950,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>152</v>
@@ -7962,7 +7962,7 @@
         <v>249</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G16" s="57" t="s">
         <v>158</v>
@@ -7979,10 +7979,10 @@
         <v>2</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>153</v>
@@ -7991,7 +7991,7 @@
         <v>1195</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>159</v>
@@ -8008,10 +8008,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>154</v>
@@ -8020,7 +8020,7 @@
         <v>1197</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>162</v>
@@ -8037,10 +8037,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>155</v>
@@ -8049,7 +8049,7 @@
         <v>253</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="G19" s="57" t="s">
         <v>157</v>
@@ -8066,10 +8066,10 @@
         <v>2</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>1526</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>1527</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>156</v>
@@ -8078,7 +8078,7 @@
         <v>623</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G20" s="57" t="s">
         <v>160</v>
@@ -8095,10 +8095,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D21" s="41" t="s">
         <v>163</v>
@@ -8107,7 +8107,7 @@
         <v>1198</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G21" s="76" t="s">
         <v>171</v>
@@ -8124,10 +8124,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>164</v>
@@ -8136,7 +8136,7 @@
         <v>624</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>170</v>
@@ -8165,7 +8165,7 @@
         <v>1169</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="G23" s="70" t="s">
         <v>62</v>
@@ -8194,7 +8194,7 @@
         <v>1170</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="G24" s="70" t="s">
         <v>1200</v>
@@ -8223,7 +8223,7 @@
         <v>1202</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="G25" s="57" t="s">
         <v>173</v>
@@ -8252,7 +8252,7 @@
         <v>1203</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>174</v>
@@ -8269,10 +8269,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>1530</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>1531</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>167</v>
@@ -8281,7 +8281,7 @@
         <v>1204</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>175</v>
@@ -8298,10 +8298,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="D28" s="38" t="s">
         <v>168</v>
@@ -8310,7 +8310,7 @@
         <v>1205</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>177</v>
@@ -8339,7 +8339,7 @@
         <v>1206</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>189</v>
@@ -8368,7 +8368,7 @@
         <v>1207</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>190</v>
@@ -8426,7 +8426,7 @@
         <v>260</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>192</v>
@@ -8455,7 +8455,7 @@
         <v>262</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>70</v>
@@ -8484,7 +8484,7 @@
         <v>264</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>193</v>
@@ -8513,7 +8513,7 @@
         <v>182</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="G35" s="70" t="s">
         <v>99</v>
@@ -8542,7 +8542,7 @@
         <v>268</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>89</v>
@@ -8571,7 +8571,7 @@
         <v>267</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>195</v>
@@ -8600,7 +8600,7 @@
         <v>271</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>196</v>
@@ -8629,7 +8629,7 @@
         <v>272</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>197</v>
@@ -8658,7 +8658,7 @@
         <v>1210</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>198</v>
@@ -8667,7 +8667,7 @@
         <v>274</v>
       </c>
       <c r="I40" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -8687,7 +8687,7 @@
         <v>275</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>199</v>
@@ -8696,7 +8696,7 @@
         <v>276</v>
       </c>
       <c r="I41" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8716,7 +8716,7 @@
         <v>188</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>115</v>
@@ -8725,7 +8725,7 @@
         <v>200</v>
       </c>
       <c r="I42" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8754,7 +8754,7 @@
         <v>204</v>
       </c>
       <c r="I43" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="11" customFormat="1" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8774,7 +8774,7 @@
         <v>1149</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="G44" s="70" t="s">
         <v>206</v>
@@ -8783,7 +8783,7 @@
         <v>291</v>
       </c>
       <c r="I44" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8803,7 +8803,7 @@
         <v>1211</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>208</v>
@@ -8832,7 +8832,7 @@
         <v>277</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>211</v>
@@ -8841,7 +8841,7 @@
         <v>278</v>
       </c>
       <c r="I46" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -8861,7 +8861,7 @@
         <v>280</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>214</v>
@@ -8870,7 +8870,7 @@
         <v>279</v>
       </c>
       <c r="I47" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -8890,7 +8890,7 @@
         <v>281</v>
       </c>
       <c r="F48" s="38" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>215</v>
@@ -8919,7 +8919,7 @@
         <v>283</v>
       </c>
       <c r="F49" s="38" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>217</v>
@@ -8948,7 +8948,7 @@
         <v>285</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>35</v>
@@ -8957,7 +8957,7 @@
         <v>286</v>
       </c>
       <c r="I50" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -8977,7 +8977,7 @@
         <v>219</v>
       </c>
       <c r="F51" s="41" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="G51" s="14" t="s">
         <v>222</v>
@@ -8986,7 +8986,7 @@
         <v>1212</v>
       </c>
       <c r="I51" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -9006,7 +9006,7 @@
         <v>221</v>
       </c>
       <c r="F52" s="38" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>223</v>
@@ -9033,7 +9033,7 @@
         <v>293</v>
       </c>
       <c r="F53" s="38" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>228</v>
@@ -9111,7 +9111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -9173,7 +9173,7 @@
         <v>1227</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>294</v>
@@ -9205,7 +9205,7 @@
         <v>296</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="G3" s="60" t="s">
         <v>297</v>
@@ -9222,10 +9222,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>107</v>
@@ -9234,7 +9234,7 @@
         <v>299</v>
       </c>
       <c r="F4" s="44" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="G4" s="61" t="s">
         <v>149</v>
@@ -9251,10 +9251,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>301</v>
@@ -9263,7 +9263,7 @@
         <v>302</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="G5" s="62" t="s">
         <v>303</v>
@@ -9295,7 +9295,7 @@
         <v>306</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>307</v>
@@ -9324,7 +9324,7 @@
         <v>1229</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G7" s="25" t="s">
         <v>310</v>
@@ -9353,7 +9353,7 @@
         <v>1230</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>68</v>
@@ -9370,10 +9370,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D9" s="44" t="s">
         <v>24</v>
@@ -9382,7 +9382,7 @@
         <v>312</v>
       </c>
       <c r="F9" s="44" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="G9" s="25" t="s">
         <v>39</v>
@@ -9399,10 +9399,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>1512</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>1513</v>
       </c>
       <c r="D10" s="44" t="s">
         <v>314</v>
@@ -9411,7 +9411,7 @@
         <v>315</v>
       </c>
       <c r="F10" s="44" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="G10" s="25" t="s">
         <v>316</v>
@@ -9440,7 +9440,7 @@
         <v>318</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="G11" s="62" t="s">
         <v>171</v>
@@ -9457,10 +9457,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>1514</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>1515</v>
       </c>
       <c r="D12" s="44" t="s">
         <v>320</v>
@@ -9469,7 +9469,7 @@
         <v>321</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="G12" s="25" t="s">
         <v>322</v>
@@ -9486,10 +9486,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>1514</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>1515</v>
       </c>
       <c r="D13" s="44" t="s">
         <v>323</v>
@@ -9498,7 +9498,7 @@
         <v>1232</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="G13" s="25" t="s">
         <v>324</v>
@@ -9515,10 +9515,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D14" s="44" t="s">
         <v>226</v>
@@ -9527,7 +9527,7 @@
         <v>1233</v>
       </c>
       <c r="F14" s="44" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="G14" s="25" t="s">
         <v>326</v>
@@ -9544,10 +9544,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>1514</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>1515</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>328</v>
@@ -9556,7 +9556,7 @@
         <v>1234</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="G15" s="62" t="s">
         <v>329</v>
@@ -9585,7 +9585,7 @@
         <v>1235</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="G16" s="60" t="s">
         <v>223</v>
@@ -9602,10 +9602,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="101" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C17" s="101" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="D17" s="102" t="s">
         <v>332</v>
@@ -9614,7 +9614,7 @@
         <v>333</v>
       </c>
       <c r="F17" s="103" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="G17" s="99" t="s">
         <v>334</v>
@@ -9631,10 +9631,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>336</v>
@@ -9643,7 +9643,7 @@
         <v>337</v>
       </c>
       <c r="F18" s="44" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="G18" s="25" t="s">
         <v>338</v>
@@ -9701,7 +9701,7 @@
         <v>344</v>
       </c>
       <c r="F20" s="44" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="G20" s="60" t="s">
         <v>345</v>
@@ -9730,7 +9730,7 @@
         <v>347</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="G21" s="25" t="s">
         <v>348</v>
@@ -9759,7 +9759,7 @@
         <v>350</v>
       </c>
       <c r="F22" s="44" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>35</v>
@@ -9788,7 +9788,7 @@
         <v>352</v>
       </c>
       <c r="F23" s="44" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="G23" s="25" t="s">
         <v>236</v>
@@ -9846,7 +9846,7 @@
         <v>359</v>
       </c>
       <c r="F25" s="44" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="G25" s="25" t="s">
         <v>360</v>
@@ -9875,7 +9875,7 @@
         <v>364</v>
       </c>
       <c r="F26" s="44" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="G26" s="25" t="s">
         <v>365</v>
@@ -9904,7 +9904,7 @@
         <v>368</v>
       </c>
       <c r="F27" s="44" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="G27" s="25" t="s">
         <v>369</v>
@@ -9933,7 +9933,7 @@
         <v>371</v>
       </c>
       <c r="F28" s="44" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>115</v>
@@ -9962,7 +9962,7 @@
         <v>374</v>
       </c>
       <c r="F29" s="44" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G29" s="81" t="s">
         <v>1156</v>
@@ -9991,7 +9991,7 @@
         <v>376</v>
       </c>
       <c r="F30" s="44" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="G30" s="25" t="s">
         <v>377</v>
@@ -10020,7 +10020,7 @@
         <v>380</v>
       </c>
       <c r="F31" s="44" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="G31" s="25" t="s">
         <v>381</v>
@@ -10049,7 +10049,7 @@
         <v>384</v>
       </c>
       <c r="F32" s="44" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="G32" s="25" t="s">
         <v>385</v>
@@ -10078,7 +10078,7 @@
         <v>387</v>
       </c>
       <c r="F33" s="72" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="G33" s="25" t="s">
         <v>388</v>
@@ -10107,7 +10107,7 @@
         <v>390</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>158</v>
@@ -10116,7 +10116,7 @@
         <v>391</v>
       </c>
       <c r="I34" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10136,7 +10136,7 @@
         <v>393</v>
       </c>
       <c r="F35" s="44" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="G35" s="25" t="s">
         <v>394</v>
@@ -10192,7 +10192,7 @@
         <v>401</v>
       </c>
       <c r="F37" s="44" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="G37" s="25" t="s">
         <v>402</v>
@@ -10219,7 +10219,7 @@
         <v>405</v>
       </c>
       <c r="F38" s="44" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="G38" s="25" t="s">
         <v>406</v>
@@ -10241,7 +10241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -10302,7 +10302,7 @@
         <v>409</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="G2" s="55" t="s">
         <v>410</v>
@@ -10311,7 +10311,7 @@
         <v>411</v>
       </c>
       <c r="I2" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="J2" s="138" t="s">
         <v>1236</v>
@@ -10334,7 +10334,7 @@
         <v>412</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="G3" s="55" t="s">
         <v>398</v>
@@ -10366,7 +10366,7 @@
         <v>617</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>414</v>
@@ -10395,7 +10395,7 @@
         <v>417</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G5" s="55" t="s">
         <v>418</v>
@@ -10482,7 +10482,7 @@
         <v>428</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G8" s="55" t="s">
         <v>429</v>
@@ -10511,7 +10511,7 @@
         <v>1150</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G9" s="74" t="s">
         <v>1151</v>
@@ -10528,10 +10528,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>433</v>
@@ -10540,7 +10540,7 @@
         <v>434</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="G10" s="55" t="s">
         <v>435</v>
@@ -10557,10 +10557,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>437</v>
@@ -10569,7 +10569,7 @@
         <v>438</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="G11" s="55" t="s">
         <v>439</v>
@@ -10586,10 +10586,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>441</v>
@@ -10598,7 +10598,7 @@
         <v>442</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="G12" s="55" t="s">
         <v>443</v>
@@ -10615,10 +10615,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>167</v>
@@ -10627,7 +10627,7 @@
         <v>445</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G13" s="55" t="s">
         <v>446</v>
@@ -10644,10 +10644,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="D14" s="38" t="s">
         <v>448</v>
@@ -10656,7 +10656,7 @@
         <v>1214</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G14" s="55" t="s">
         <v>449</v>
@@ -10673,10 +10673,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>451</v>
@@ -10685,7 +10685,7 @@
         <v>452</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="G15" s="55" t="s">
         <v>453</v>
@@ -10714,7 +10714,7 @@
         <v>456</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="G16" s="55" t="s">
         <v>457</v>
@@ -10731,10 +10731,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>459</v>
@@ -10743,7 +10743,7 @@
         <v>460</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="G17" s="55" t="s">
         <v>461</v>
@@ -10760,10 +10760,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C18" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>367</v>
@@ -10772,7 +10772,7 @@
         <v>463</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="G18" s="55" t="s">
         <v>369</v>
@@ -10789,10 +10789,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>465</v>
@@ -10801,7 +10801,7 @@
         <v>1215</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="G19" s="55" t="s">
         <v>466</v>
@@ -10830,7 +10830,7 @@
         <v>1217</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="G20" s="55" t="s">
         <v>469</v>
@@ -10839,7 +10839,7 @@
         <v>1216</v>
       </c>
       <c r="I20" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -10847,10 +10847,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C21" s="38" t="s">
         <v>1541</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>1542</v>
       </c>
       <c r="D21" s="39" t="s">
         <v>24</v>
@@ -10859,7 +10859,7 @@
         <v>470</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="G21" s="55" t="s">
         <v>39</v>
@@ -10876,10 +10876,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C22" s="38" t="s">
         <v>1541</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>1542</v>
       </c>
       <c r="D22" s="39" t="s">
         <v>472</v>
@@ -10888,7 +10888,7 @@
         <v>1218</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="G22" s="55" t="s">
         <v>473</v>
@@ -10917,7 +10917,7 @@
         <v>1219</v>
       </c>
       <c r="F23" s="39" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="G23" s="55" t="s">
         <v>356</v>
@@ -10926,7 +10926,7 @@
         <v>475</v>
       </c>
       <c r="I23" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -10946,7 +10946,7 @@
         <v>477</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="G24" s="55" t="s">
         <v>478</v>
@@ -10975,7 +10975,7 @@
         <v>481</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="G25" s="55" t="s">
         <v>482</v>
@@ -10984,7 +10984,7 @@
         <v>483</v>
       </c>
       <c r="I25" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -11013,7 +11013,7 @@
         <v>487</v>
       </c>
       <c r="I26" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -11062,7 +11062,7 @@
         <v>489</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="G28" s="55" t="s">
         <v>115</v>
@@ -11091,7 +11091,7 @@
         <v>491</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="G29" s="55" t="s">
         <v>492</v>
@@ -11120,7 +11120,7 @@
         <v>1223</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="G30" s="64" t="s">
         <v>47</v>
@@ -11129,7 +11129,7 @@
         <v>1222</v>
       </c>
       <c r="I30" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -11149,7 +11149,7 @@
         <v>494</v>
       </c>
       <c r="F31" s="46" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="G31" s="55" t="s">
         <v>35</v>
@@ -11158,7 +11158,7 @@
         <v>495</v>
       </c>
       <c r="I31" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="225" x14ac:dyDescent="0.25">
@@ -11187,7 +11187,7 @@
         <v>496</v>
       </c>
       <c r="I32" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -11236,7 +11236,7 @@
         <v>502</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="G34" s="55" t="s">
         <v>503</v>
@@ -11265,7 +11265,7 @@
         <v>506</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="G35" s="55" t="s">
         <v>507</v>
@@ -11274,7 +11274,7 @@
         <v>508</v>
       </c>
       <c r="I35" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -11294,7 +11294,7 @@
         <v>1225</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="G36" s="55" t="s">
         <v>510</v>
@@ -11303,7 +11303,7 @@
         <v>511</v>
       </c>
       <c r="I36" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -11323,7 +11323,7 @@
         <v>512</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="G37" s="55" t="s">
         <v>229</v>
@@ -11332,7 +11332,7 @@
         <v>513</v>
       </c>
       <c r="I37" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -11410,7 +11410,7 @@
         <v>522</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="G40" s="55" t="s">
         <v>523</v>
@@ -11437,7 +11437,7 @@
         <v>525</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="G41" s="55" t="s">
         <v>71</v>
@@ -11464,7 +11464,7 @@
         <v>528</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="G42" s="55" t="s">
         <v>529</v>
@@ -11486,7 +11486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -11536,10 +11536,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>1543</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>1544</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>97</v>
@@ -11548,7 +11548,7 @@
         <v>531</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>101</v>
@@ -11580,7 +11580,7 @@
         <v>533</v>
       </c>
       <c r="F3" s="51" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G3" s="55" t="s">
         <v>60</v>
@@ -11612,7 +11612,7 @@
         <v>1272</v>
       </c>
       <c r="F4" s="51" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="G4" s="55" t="s">
         <v>71</v>
@@ -11641,7 +11641,7 @@
         <v>536</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G5" s="55" t="s">
         <v>537</v>
@@ -11728,7 +11728,7 @@
         <v>544</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>307</v>
@@ -11757,7 +11757,7 @@
         <v>545</v>
       </c>
       <c r="F9" s="51" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>425</v>
@@ -11774,10 +11774,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>185</v>
@@ -11786,7 +11786,7 @@
         <v>547</v>
       </c>
       <c r="F10" s="51" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>548</v>
@@ -11795,7 +11795,7 @@
         <v>1274</v>
       </c>
       <c r="I10" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -11803,10 +11803,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>437</v>
@@ -11832,10 +11832,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>24</v>
@@ -11844,7 +11844,7 @@
         <v>551</v>
       </c>
       <c r="F12" s="51" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>39</v>
@@ -11861,10 +11861,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>553</v>
@@ -11873,7 +11873,7 @@
         <v>554</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="G13" s="55" t="s">
         <v>555</v>
@@ -11902,7 +11902,7 @@
         <v>557</v>
       </c>
       <c r="F14" s="51" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>558</v>
@@ -11919,10 +11919,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>472</v>
@@ -11948,10 +11948,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>562</v>
@@ -11977,10 +11977,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>367</v>
@@ -11989,7 +11989,7 @@
         <v>1276</v>
       </c>
       <c r="F17" s="51" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="G17" s="55" t="s">
         <v>369</v>
@@ -12018,7 +12018,7 @@
         <v>566</v>
       </c>
       <c r="F18" s="51" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>338</v>
@@ -12027,7 +12027,7 @@
         <v>567</v>
       </c>
       <c r="I18" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -12035,10 +12035,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>1547</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>1548</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>568</v>
@@ -12047,7 +12047,7 @@
         <v>571</v>
       </c>
       <c r="F19" s="51" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>569</v>
@@ -12064,10 +12064,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C20" s="41" t="s">
         <v>1547</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>1548</v>
       </c>
       <c r="D20" s="41" t="s">
         <v>133</v>
@@ -12076,7 +12076,7 @@
         <v>572</v>
       </c>
       <c r="F20" s="134" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="G20" s="64" t="s">
         <v>142</v>
@@ -12093,10 +12093,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>354</v>
@@ -12105,7 +12105,7 @@
         <v>574</v>
       </c>
       <c r="F21" s="51" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>356</v>
@@ -12122,10 +12122,10 @@
         <v>5</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>105</v>
@@ -12134,7 +12134,7 @@
         <v>576</v>
       </c>
       <c r="F22" s="51" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="G22" s="55" t="s">
         <v>1147</v>
@@ -12192,7 +12192,7 @@
         <v>621</v>
       </c>
       <c r="F24" s="135" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G24" s="76" t="s">
         <v>1152</v>
@@ -12221,7 +12221,7 @@
         <v>581</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="G25" s="55" t="s">
         <v>582</v>
@@ -12230,7 +12230,7 @@
         <v>1277</v>
       </c>
       <c r="I25" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -12250,7 +12250,7 @@
         <v>583</v>
       </c>
       <c r="F26" s="51" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="G26" s="55" t="s">
         <v>47</v>
@@ -12279,7 +12279,7 @@
         <v>585</v>
       </c>
       <c r="F27" s="51" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G27" s="55" t="s">
         <v>13</v>
@@ -12308,7 +12308,7 @@
         <v>588</v>
       </c>
       <c r="F28" s="51" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="G28" s="74" t="s">
         <v>1280</v>
@@ -12335,7 +12335,7 @@
         <v>590</v>
       </c>
       <c r="F29" s="51" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="G29" s="66" t="s">
         <v>591</v>
@@ -12344,7 +12344,7 @@
         <v>592</v>
       </c>
       <c r="I29" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="120" x14ac:dyDescent="0.25">
@@ -12362,7 +12362,7 @@
         <v>594</v>
       </c>
       <c r="F30" s="51" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>595</v>
@@ -12398,7 +12398,7 @@
         <v>600</v>
       </c>
       <c r="I31" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="J31" s="138" t="s">
         <v>1236</v>
@@ -12419,7 +12419,7 @@
         <v>1278</v>
       </c>
       <c r="F32" s="51" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="G32" s="55" t="s">
         <v>602</v>
@@ -12428,7 +12428,7 @@
         <v>603</v>
       </c>
       <c r="I32" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -12448,7 +12448,7 @@
         <v>604</v>
       </c>
       <c r="F33" s="51" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="G33" s="55" t="s">
         <v>605</v>
@@ -12457,7 +12457,7 @@
         <v>1279</v>
       </c>
       <c r="I33" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>608</v>
       </c>
       <c r="F35" s="51" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="G35" s="55" t="s">
         <v>523</v>
@@ -12535,7 +12535,7 @@
         <v>610</v>
       </c>
       <c r="F36" s="90" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>360</v>
@@ -12557,7 +12557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -12613,10 +12613,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E2" s="51" t="s">
         <v>87</v>
@@ -12625,7 +12625,7 @@
         <v>735</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="H2" s="55" t="s">
         <v>89</v>
@@ -12648,10 +12648,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="140" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D3" s="141" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="E3" s="141" t="s">
         <v>696</v>
@@ -12660,7 +12660,7 @@
         <v>697</v>
       </c>
       <c r="G3" s="141" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="H3" s="143" t="s">
         <v>698</v>
@@ -12692,7 +12692,7 @@
         <v>700</v>
       </c>
       <c r="G4" s="51" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="H4" s="55" t="s">
         <v>701</v>
@@ -12724,7 +12724,7 @@
         <v>703</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="H5" s="55" t="s">
         <v>398</v>
@@ -12788,7 +12788,7 @@
         <v>705</v>
       </c>
       <c r="G7" s="51" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="H7" s="55" t="s">
         <v>706</v>
@@ -12820,7 +12820,7 @@
         <v>709</v>
       </c>
       <c r="G8" s="51" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="H8" s="55" t="s">
         <v>710</v>
@@ -12916,7 +12916,7 @@
         <v>719</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="H11" s="55" t="s">
         <v>720</v>
@@ -12948,7 +12948,7 @@
         <v>740</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>360</v>
@@ -13012,7 +13012,7 @@
         <v>723</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>537</v>
@@ -13044,7 +13044,7 @@
         <v>725</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="H15" s="55" t="s">
         <v>540</v>
@@ -13064,10 +13064,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="E16" s="68" t="s">
         <v>727</v>
@@ -13076,7 +13076,7 @@
         <v>742</v>
       </c>
       <c r="G16" s="51" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="H16" s="74" t="s">
         <v>1155</v>
@@ -13096,10 +13096,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="E17" s="38" t="s">
         <v>728</v>
@@ -13108,7 +13108,7 @@
         <v>744</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="H17" s="55" t="s">
         <v>729</v>
@@ -13128,10 +13128,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>627</v>
@@ -13140,7 +13140,7 @@
         <v>628</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="H18" s="55" t="s">
         <v>629</v>
@@ -13160,10 +13160,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E19" s="38" t="s">
         <v>140</v>
@@ -13172,7 +13172,7 @@
         <v>631</v>
       </c>
       <c r="G19" s="51" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>151</v>
@@ -13204,7 +13204,7 @@
         <v>746</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="H20" s="55" t="s">
         <v>634</v>
@@ -13224,10 +13224,10 @@
         <v>6</v>
       </c>
       <c r="C21" s="38" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D21" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="E21" s="38" t="s">
         <v>635</v>
@@ -13236,7 +13236,7 @@
         <v>636</v>
       </c>
       <c r="G21" s="51" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>637</v>
@@ -13256,10 +13256,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="38" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D22" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="E22" s="41" t="s">
         <v>638</v>
@@ -13268,7 +13268,7 @@
         <v>749</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H22" s="64" t="s">
         <v>639</v>
@@ -13288,10 +13288,10 @@
         <v>6</v>
       </c>
       <c r="C23" s="38" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="E23" s="38" t="s">
         <v>640</v>
@@ -13300,7 +13300,7 @@
         <v>641</v>
       </c>
       <c r="G23" s="51" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="H23" s="55" t="s">
         <v>642</v>
@@ -13332,7 +13332,7 @@
         <v>645</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>646</v>
@@ -13364,7 +13364,7 @@
         <v>649</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>650</v>
@@ -13373,7 +13373,7 @@
         <v>651</v>
       </c>
       <c r="J25" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -13428,7 +13428,7 @@
         <v>654</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="H27" s="55" t="s">
         <v>655</v>
@@ -13460,7 +13460,7 @@
         <v>751</v>
       </c>
       <c r="G28" s="38" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="H28" s="57" t="s">
         <v>658</v>
@@ -13492,7 +13492,7 @@
         <v>660</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>661</v>
@@ -13524,7 +13524,7 @@
         <v>753</v>
       </c>
       <c r="G30" s="104" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="H30" s="119" t="s">
         <v>664</v>
@@ -13556,7 +13556,7 @@
         <v>666</v>
       </c>
       <c r="G31" s="38" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H31" s="55" t="s">
         <v>667</v>
@@ -13588,7 +13588,7 @@
         <v>670</v>
       </c>
       <c r="G32" s="38" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="H32" s="55" t="s">
         <v>671</v>
@@ -13620,7 +13620,7 @@
         <v>755</v>
       </c>
       <c r="G33" s="38" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>674</v>
@@ -13661,7 +13661,7 @@
         <v>677</v>
       </c>
       <c r="J34" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -13684,7 +13684,7 @@
         <v>679</v>
       </c>
       <c r="G35" s="38" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="H35" s="55" t="s">
         <v>680</v>
@@ -13716,7 +13716,7 @@
         <v>683</v>
       </c>
       <c r="G36" s="38" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>684</v>
@@ -13748,7 +13748,7 @@
         <v>757</v>
       </c>
       <c r="G37" s="51" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="H37" s="67" t="s">
         <v>686</v>
@@ -13780,7 +13780,7 @@
         <v>759</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="H38" s="55" t="s">
         <v>687</v>
@@ -13789,7 +13789,7 @@
         <v>1285</v>
       </c>
       <c r="J38" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -13812,7 +13812,7 @@
         <v>1176</v>
       </c>
       <c r="G39" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="H39" s="74" t="s">
         <v>99</v>
@@ -13844,7 +13844,7 @@
         <v>760</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>117</v>
@@ -13853,7 +13853,7 @@
         <v>761</v>
       </c>
       <c r="J40" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -13876,7 +13876,7 @@
         <v>690</v>
       </c>
       <c r="G41" s="38" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>125</v>
@@ -13885,7 +13885,7 @@
         <v>691</v>
       </c>
       <c r="J41" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -13917,7 +13917,7 @@
         <v>695</v>
       </c>
       <c r="J42" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -13949,7 +13949,7 @@
         <v>731</v>
       </c>
       <c r="J43" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -13972,7 +13972,7 @@
         <v>762</v>
       </c>
       <c r="G44" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>307</v>
@@ -14002,7 +14002,7 @@
         <v>732</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="H45" s="55" t="s">
         <v>58</v>
@@ -14032,7 +14032,7 @@
         <v>765</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="H46" s="55" t="s">
         <v>734</v>
@@ -14041,7 +14041,7 @@
         <v>766</v>
       </c>
       <c r="J46" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -14058,7 +14058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -14143,10 +14143,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="D3" s="38" t="s">
         <v>768</v>
@@ -14155,7 +14155,7 @@
         <v>769</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="G3" s="55" t="s">
         <v>770</v>
@@ -14175,10 +14175,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>1543</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>1544</v>
       </c>
       <c r="D4" s="38" t="s">
         <v>771</v>
@@ -14187,7 +14187,7 @@
         <v>772</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G4" s="55" t="s">
         <v>773</v>
@@ -14236,10 +14236,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="D6" s="38" t="s">
         <v>738</v>
@@ -14315,7 +14315,7 @@
         <v>916</v>
       </c>
       <c r="I8" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -14344,7 +14344,7 @@
         <v>914</v>
       </c>
       <c r="I9" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -14373,7 +14373,7 @@
         <v>786</v>
       </c>
       <c r="I10" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="135" x14ac:dyDescent="0.25">
@@ -14393,7 +14393,7 @@
         <v>917</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="G11" s="55" t="s">
         <v>788</v>
@@ -14402,7 +14402,7 @@
         <v>918</v>
       </c>
       <c r="I11" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -14422,7 +14422,7 @@
         <v>919</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G12" s="55" t="s">
         <v>790</v>
@@ -14451,7 +14451,7 @@
         <v>921</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G13" s="55" t="s">
         <v>792</v>
@@ -14480,7 +14480,7 @@
         <v>923</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G14" s="55" t="s">
         <v>193</v>
@@ -14497,10 +14497,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="30" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>1560</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>1561</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>793</v>
@@ -14538,7 +14538,7 @@
         <v>925</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="G16" s="55" t="s">
         <v>686</v>
@@ -14567,7 +14567,7 @@
         <v>797</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="G17" s="55" t="s">
         <v>141</v>
@@ -14584,10 +14584,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>799</v>
@@ -14596,7 +14596,7 @@
         <v>926</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="G18" s="55" t="s">
         <v>800</v>
@@ -14613,10 +14613,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>801</v>
@@ -14625,7 +14625,7 @@
         <v>928</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G19" s="55" t="s">
         <v>802</v>
@@ -14642,10 +14642,10 @@
         <v>7</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>648</v>
@@ -14654,7 +14654,7 @@
         <v>803</v>
       </c>
       <c r="F20" s="38" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G20" s="55" t="s">
         <v>650</v>
@@ -14663,7 +14663,7 @@
         <v>1251</v>
       </c>
       <c r="I20" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -14671,10 +14671,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>804</v>
@@ -14683,7 +14683,7 @@
         <v>930</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="G21" s="55" t="s">
         <v>805</v>
@@ -14700,10 +14700,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>806</v>
@@ -14712,7 +14712,7 @@
         <v>1253</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G22" s="55" t="s">
         <v>807</v>
@@ -14729,10 +14729,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>809</v>
@@ -14741,7 +14741,7 @@
         <v>810</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G23" s="55" t="s">
         <v>811</v>
@@ -14770,7 +14770,7 @@
         <v>931</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="G24" s="55" t="s">
         <v>674</v>
@@ -14787,10 +14787,10 @@
         <v>7</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D25" s="38" t="s">
         <v>813</v>
@@ -14799,7 +14799,7 @@
         <v>933</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G25" s="55" t="s">
         <v>814</v>
@@ -14816,10 +14816,10 @@
         <v>7</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D26" s="38" t="s">
         <v>815</v>
@@ -14828,7 +14828,7 @@
         <v>816</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="G26" s="55" t="s">
         <v>817</v>
@@ -14845,10 +14845,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="D27" s="38" t="s">
         <v>818</v>
@@ -14857,7 +14857,7 @@
         <v>1254</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="G27" s="55" t="s">
         <v>819</v>
@@ -14886,7 +14886,7 @@
         <v>937</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="G28" s="55" t="s">
         <v>820</v>
@@ -14903,10 +14903,10 @@
         <v>7</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="D29" s="38" t="s">
         <v>821</v>
@@ -14915,7 +14915,7 @@
         <v>822</v>
       </c>
       <c r="F29" s="51" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="G29" s="57" t="s">
         <v>823</v>
@@ -14924,7 +14924,7 @@
         <v>824</v>
       </c>
       <c r="I29" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -14932,10 +14932,10 @@
         <v>7</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>825</v>
@@ -14944,7 +14944,7 @@
         <v>939</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="G30" s="55" t="s">
         <v>826</v>
@@ -14953,7 +14953,7 @@
         <v>940</v>
       </c>
       <c r="I30" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -14961,10 +14961,10 @@
         <v>7</v>
       </c>
       <c r="B31" s="30" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>1567</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>1568</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>827</v>
@@ -14973,7 +14973,7 @@
         <v>1255</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="G31" s="55" t="s">
         <v>828</v>
@@ -14990,10 +14990,10 @@
         <v>7</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="D32" s="38" t="s">
         <v>829</v>
@@ -15002,7 +15002,7 @@
         <v>942</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="G32" s="55" t="s">
         <v>830</v>
@@ -15011,7 +15011,7 @@
         <v>1256</v>
       </c>
       <c r="I32" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -15031,7 +15031,7 @@
         <v>944</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="G33" s="84" t="s">
         <v>1159</v>
@@ -15048,10 +15048,10 @@
         <v>7</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>943</v>
@@ -15089,7 +15089,7 @@
         <v>948</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="G35" s="55" t="s">
         <v>834</v>
@@ -15106,10 +15106,10 @@
         <v>7</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>835</v>
@@ -15118,7 +15118,7 @@
         <v>836</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="G36" s="55" t="s">
         <v>837</v>
@@ -15147,7 +15147,7 @@
         <v>949</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="G37" s="55" t="s">
         <v>840</v>
@@ -15205,7 +15205,7 @@
         <v>951</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="G39" s="55" t="s">
         <v>844</v>
@@ -15234,7 +15234,7 @@
         <v>846</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="G40" s="83" t="s">
         <v>1157</v>
@@ -15263,7 +15263,7 @@
         <v>1261</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G41" s="55" t="s">
         <v>1260</v>
@@ -15272,7 +15272,7 @@
         <v>953</v>
       </c>
       <c r="I41" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -15292,7 +15292,7 @@
         <v>848</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G42" s="55" t="s">
         <v>850</v>
@@ -15321,7 +15321,7 @@
         <v>1262</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="G43" s="55" t="s">
         <v>853</v>
@@ -15350,7 +15350,7 @@
         <v>855</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="G44" s="55" t="s">
         <v>856</v>
@@ -15359,7 +15359,7 @@
         <v>857</v>
       </c>
       <c r="I44" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="11" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -15379,7 +15379,7 @@
         <v>955</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="G45" s="14" t="s">
         <v>859</v>
@@ -15388,7 +15388,7 @@
         <v>1263</v>
       </c>
       <c r="I45" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -15408,7 +15408,7 @@
         <v>956</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="G46" s="55" t="s">
         <v>861</v>
@@ -15417,7 +15417,7 @@
         <v>957</v>
       </c>
       <c r="I46" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="135" x14ac:dyDescent="0.25">
@@ -15437,7 +15437,7 @@
         <v>958</v>
       </c>
       <c r="F47" s="46" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="G47" s="86" t="s">
         <v>720</v>
@@ -15446,7 +15446,7 @@
         <v>1160</v>
       </c>
       <c r="I47" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -15466,7 +15466,7 @@
         <v>959</v>
       </c>
       <c r="F48" s="38" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>863</v>
@@ -15475,7 +15475,7 @@
         <v>960</v>
       </c>
       <c r="I48" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="150" x14ac:dyDescent="0.25">
@@ -15495,7 +15495,7 @@
         <v>961</v>
       </c>
       <c r="F49" s="38" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>865</v>
@@ -15504,7 +15504,7 @@
         <v>1264</v>
       </c>
       <c r="I49" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -15524,7 +15524,7 @@
         <v>962</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="G50" s="55" t="s">
         <v>867</v>
@@ -15533,7 +15533,7 @@
         <v>963</v>
       </c>
       <c r="I50" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -15553,7 +15553,7 @@
         <v>869</v>
       </c>
       <c r="F51" s="38" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>870</v>
@@ -15562,7 +15562,7 @@
         <v>871</v>
       </c>
       <c r="I51" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -15582,7 +15582,7 @@
         <v>1265</v>
       </c>
       <c r="F52" s="38" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G52" s="55" t="s">
         <v>873</v>
@@ -15591,7 +15591,7 @@
         <v>964</v>
       </c>
       <c r="I52" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -15692,7 +15692,7 @@
         <v>969</v>
       </c>
       <c r="F56" s="38" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="G56" s="55" t="s">
         <v>93</v>
@@ -15719,7 +15719,7 @@
         <v>880</v>
       </c>
       <c r="F57" s="38" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="G57" s="55" t="s">
         <v>117</v>
@@ -15773,7 +15773,7 @@
         <v>974</v>
       </c>
       <c r="F59" s="38" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="G59" s="87" t="s">
         <v>698</v>
@@ -15881,7 +15881,7 @@
         <v>976</v>
       </c>
       <c r="F63" s="38" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>887</v>
@@ -15908,7 +15908,7 @@
         <v>889</v>
       </c>
       <c r="F64" s="38" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="G64" s="55" t="s">
         <v>890</v>
@@ -15935,7 +15935,7 @@
         <v>978</v>
       </c>
       <c r="F65" s="38" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="G65" s="55" t="s">
         <v>1269</v>
@@ -15962,7 +15962,7 @@
         <v>1270</v>
       </c>
       <c r="F66" s="38" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="G66" s="55" t="s">
         <v>894</v>
@@ -16043,7 +16043,7 @@
         <v>902</v>
       </c>
       <c r="F69" s="38" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>903</v>
@@ -16097,7 +16097,7 @@
         <v>985</v>
       </c>
       <c r="F71" s="38" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="G71" s="55" t="s">
         <v>910</v>
@@ -16182,8 +16182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16276,7 +16276,7 @@
         <v>991</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="G3" s="47" t="s">
         <v>992</v>
@@ -16305,7 +16305,7 @@
         <v>1177</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="G4" s="47" t="s">
         <v>995</v>
@@ -16363,7 +16363,7 @@
         <v>1120</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G6" s="47" t="s">
         <v>984</v>
@@ -16380,10 +16380,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D7" s="38" t="s">
         <v>633</v>
@@ -16392,7 +16392,7 @@
         <v>1287</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G7" s="47" t="s">
         <v>998</v>
@@ -16409,10 +16409,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D8" s="38" t="s">
         <v>999</v>
@@ -16421,7 +16421,7 @@
         <v>1123</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="G8" s="47" t="s">
         <v>1000</v>
@@ -16430,7 +16430,7 @@
         <v>1288</v>
       </c>
       <c r="I8" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -16438,10 +16438,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D9" s="38" t="s">
         <v>1001</v>
@@ -16450,7 +16450,7 @@
         <v>1002</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G9" s="73" t="s">
         <v>1162</v>
@@ -16467,10 +16467,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="38" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>1571</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>1572</v>
       </c>
       <c r="D10" s="38" t="s">
         <v>1003</v>
@@ -16479,7 +16479,7 @@
         <v>1124</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="G10" s="47" t="s">
         <v>1004</v>
@@ -16496,10 +16496,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D11" s="38" t="s">
         <v>1005</v>
@@ -16508,7 +16508,7 @@
         <v>1289</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="G11" s="47" t="s">
         <v>1006</v>
@@ -16525,10 +16525,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D12" s="38" t="s">
         <v>14</v>
@@ -16537,7 +16537,7 @@
         <v>1008</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G12" s="47" t="s">
         <v>29</v>
@@ -16554,10 +16554,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D13" s="38" t="s">
         <v>1010</v>
@@ -16566,7 +16566,7 @@
         <v>1011</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G13" s="47" t="s">
         <v>1012</v>
@@ -16583,10 +16583,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="38" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>1514</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>1515</v>
       </c>
       <c r="D14" s="38" t="s">
         <v>1014</v>
@@ -16595,7 +16595,7 @@
         <v>1290</v>
       </c>
       <c r="F14" s="38" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="G14" s="47" t="s">
         <v>1015</v>
@@ -16612,10 +16612,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D15" s="38" t="s">
         <v>156</v>
@@ -16624,7 +16624,7 @@
         <v>1291</v>
       </c>
       <c r="F15" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G15" s="47" t="s">
         <v>160</v>
@@ -16641,10 +16641,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>121</v>
@@ -16653,7 +16653,7 @@
         <v>1017</v>
       </c>
       <c r="F16" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G16" s="47" t="s">
         <v>127</v>
@@ -16670,10 +16670,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>682</v>
@@ -16682,7 +16682,7 @@
         <v>1019</v>
       </c>
       <c r="F17" s="38" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G17" s="47" t="s">
         <v>684</v>
@@ -16699,10 +16699,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D18" s="38" t="s">
         <v>1021</v>
@@ -16728,10 +16728,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>640</v>
@@ -16757,10 +16757,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D20" s="38" t="s">
         <v>712</v>
@@ -16786,10 +16786,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>895</v>
@@ -16815,10 +16815,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>1031</v>
@@ -16844,10 +16844,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>644</v>
@@ -16873,10 +16873,10 @@
         <v>8</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D24" s="121" t="s">
         <v>535</v>
@@ -16902,10 +16902,10 @@
         <v>8</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="D25" s="38" t="s">
         <v>362</v>
@@ -16914,7 +16914,7 @@
         <v>1294</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="G25" s="47" t="s">
         <v>701</v>
@@ -16931,10 +16931,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="D26" s="38" t="s">
         <v>396</v>
@@ -16943,7 +16943,7 @@
         <v>1127</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="G26" s="47" t="s">
         <v>398</v>
@@ -16972,7 +16972,7 @@
         <v>1038</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="G27" s="47" t="s">
         <v>1039</v>
@@ -16981,7 +16981,7 @@
         <v>1030</v>
       </c>
       <c r="I27" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="105" x14ac:dyDescent="0.25">
@@ -16989,10 +16989,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D28" s="38" t="s">
         <v>1040</v>
@@ -17001,7 +17001,7 @@
         <v>1129</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="G28" s="47" t="s">
         <v>1041</v>
@@ -17018,10 +17018,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="D29" s="38" t="s">
         <v>653</v>
@@ -17030,7 +17030,7 @@
         <v>1042</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="G29" s="47" t="s">
         <v>655</v>
@@ -17047,10 +17047,10 @@
         <v>8</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>1044</v>
@@ -17076,10 +17076,10 @@
         <v>8</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D31" s="41" t="s">
         <v>181</v>
@@ -17097,7 +17097,7 @@
         <v>1296</v>
       </c>
       <c r="I31" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -17105,10 +17105,10 @@
         <v>8</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D32" s="38" t="s">
         <v>154</v>
@@ -17117,7 +17117,7 @@
         <v>1297</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="G32" s="47" t="s">
         <v>162</v>
@@ -17134,10 +17134,10 @@
         <v>8</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D33" s="46" t="s">
         <v>1048</v>
@@ -17155,7 +17155,7 @@
         <v>1165</v>
       </c>
       <c r="I33" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -17163,10 +17163,10 @@
         <v>8</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>829</v>
@@ -17192,10 +17192,10 @@
         <v>8</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>833</v>
@@ -17221,10 +17221,10 @@
         <v>8</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>1054</v>
@@ -17242,7 +17242,7 @@
         <v>1057</v>
       </c>
       <c r="I36" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -17250,10 +17250,10 @@
         <v>8</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>1058</v>
@@ -17262,7 +17262,7 @@
         <v>1059</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G37" s="47" t="s">
         <v>1060</v>
@@ -17279,10 +17279,10 @@
         <v>8</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>1062</v>
@@ -17291,7 +17291,7 @@
         <v>1298</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="G38" s="47" t="s">
         <v>1063</v>
@@ -17320,7 +17320,7 @@
         <v>1065</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="G39" s="38" t="s">
         <v>1066</v>
@@ -17465,7 +17465,7 @@
         <v>1300</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="G44" s="47" t="s">
         <v>37</v>
@@ -17494,7 +17494,7 @@
         <v>1080</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>885</v>
@@ -17523,7 +17523,7 @@
         <v>1082</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="G46" s="47" t="s">
         <v>128</v>
@@ -17552,7 +17552,7 @@
         <v>1133</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="G47" s="47" t="s">
         <v>1085</v>
@@ -17561,7 +17561,7 @@
         <v>1134</v>
       </c>
       <c r="I47" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="210" x14ac:dyDescent="0.25">
@@ -17581,7 +17581,7 @@
         <v>1135</v>
       </c>
       <c r="F48" s="38" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="G48" s="47" t="s">
         <v>11</v>
@@ -17590,7 +17590,7 @@
         <v>1136</v>
       </c>
       <c r="I48" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -17619,7 +17619,7 @@
         <v>1187</v>
       </c>
       <c r="I49" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -17639,7 +17639,7 @@
         <v>1088</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="G50" s="38" t="s">
         <v>177</v>
@@ -17648,7 +17648,7 @@
         <v>1089</v>
       </c>
       <c r="I50" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -17668,7 +17668,7 @@
         <v>1090</v>
       </c>
       <c r="F51" s="38" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="G51" s="47" t="s">
         <v>1091</v>
@@ -17677,7 +17677,7 @@
         <v>1092</v>
       </c>
       <c r="I51" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -17706,7 +17706,7 @@
         <v>1095</v>
       </c>
       <c r="I52" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -17726,7 +17726,7 @@
         <v>1096</v>
       </c>
       <c r="F53" s="38" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="G53" s="38" t="s">
         <v>983</v>
@@ -17755,7 +17755,7 @@
         <v>1175</v>
       </c>
       <c r="F54" s="38" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="G54" s="47" t="s">
         <v>117</v>
@@ -17784,7 +17784,7 @@
         <v>1099</v>
       </c>
       <c r="F55" s="38" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="G55" s="47" t="s">
         <v>1100</v>
@@ -17842,7 +17842,7 @@
         <v>1137</v>
       </c>
       <c r="F57" s="38" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="G57" s="47" t="s">
         <v>1106</v>
@@ -17851,7 +17851,7 @@
         <v>1138</v>
       </c>
       <c r="I57" s="137" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -17871,7 +17871,7 @@
         <v>1108</v>
       </c>
       <c r="F58" s="38" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="G58" s="47" t="s">
         <v>1109</v>
@@ -17900,7 +17900,7 @@
         <v>1112</v>
       </c>
       <c r="F59" s="38" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="G59" s="47" t="s">
         <v>1113</v>

</xml_diff>